<commit_message>
Test data file 6th jan
data file after flushing the database
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -63,21 +63,6 @@
     <t>invoice desc 1</t>
   </si>
   <si>
-    <t>Bank Charges</t>
-  </si>
-  <si>
-    <t>inv desc 2</t>
-  </si>
-  <si>
-    <t>measure 1</t>
-  </si>
-  <si>
-    <t>Hi !!</t>
-  </si>
-  <si>
-    <t>invoice memo</t>
-  </si>
-  <si>
     <t>NetchainTest.InvoiceListVendor</t>
   </si>
   <si>
@@ -141,49 +126,62 @@
     <t>notes12345</t>
   </si>
   <si>
+    <t>9098989912</t>
+  </si>
+  <si>
+    <t>8178789909</t>
+  </si>
+  <si>
+    <t>Qwerty@123</t>
+  </si>
+  <si>
+    <t>Dell</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Vendor 1</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>ruchira.m</t>
+  </si>
+  <si>
+    <t>ruchira.m,1234</t>
+  </si>
+  <si>
+    <t>Amanora</t>
+  </si>
+  <si>
     <t>bangalore</t>
   </si>
   <si>
-    <t>bang dept 1</t>
-  </si>
-  <si>
-    <t>9098989912</t>
-  </si>
-  <si>
-    <t>8178789909</t>
-  </si>
-  <si>
-    <t>Qwerty@123</t>
-  </si>
-  <si>
-    <t>ruchira94</t>
-  </si>
-  <si>
-    <t>ruchira94,1234</t>
-  </si>
-  <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>laptop</t>
+    <t>NetChain2-AP New: Invoice</t>
+  </si>
+  <si>
+    <t>test product</t>
+  </si>
+  <si>
+    <t>inv desc2</t>
+  </si>
+  <si>
+    <t>measure1</t>
+  </si>
+  <si>
+    <t>message1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,17 +204,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -532,10 +527,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -543,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -554,13 +549,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -595,13 +590,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -613,118 +608,124 @@
         <v>500</v>
       </c>
       <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>50</v>
       </c>
       <c r="M4">
-        <v>4.5555500000000002</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>10.44444</v>
       </c>
       <c r="O4" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>42</v>
       </c>
       <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" t="s">
         <v>32</v>
       </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" t="s">
-        <v>37</v>
-      </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="Q7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="R7">
         <v>411099</v>
       </c>
       <c r="S7" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="V7">
         <v>12345</v>
       </c>
       <c r="W7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="X7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest changes for demo
tfft
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -84,15 +84,6 @@
     <t>other</t>
   </si>
   <si>
-    <t>ltd</t>
-  </si>
-  <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>Maharashtra</t>
-  </si>
-  <si>
     <t>Tech Mahindra</t>
   </si>
   <si>
@@ -105,33 +96,6 @@
     <t>Ms</t>
   </si>
   <si>
-    <t>Parul</t>
-  </si>
-  <si>
-    <t>Gupta</t>
-  </si>
-  <si>
-    <t>Tata Technologies</t>
-  </si>
-  <si>
-    <t>phase3</t>
-  </si>
-  <si>
-    <t>rmhaisurkar@gmail.com</t>
-  </si>
-  <si>
-    <t>www.tata.com</t>
-  </si>
-  <si>
-    <t>notes12345</t>
-  </si>
-  <si>
-    <t>9098989912</t>
-  </si>
-  <si>
-    <t>8178789909</t>
-  </si>
-  <si>
     <t>Qwerty@123</t>
   </si>
   <si>
@@ -172,6 +136,93 @@
   </si>
   <si>
     <t>message1</t>
+  </si>
+  <si>
+    <t>Bank Charges</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Xyz</t>
+  </si>
+  <si>
+    <t>Inc</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>demotest@gmail.com</t>
+  </si>
+  <si>
+    <t>www.microsoft.com</t>
+  </si>
+  <si>
+    <t>other1234</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>NetChain2 – AP Vendor: New</t>
+  </si>
+  <si>
+    <t>NetchainTest.CreateVendorNeg</t>
+  </si>
+  <si>
+    <t>www.facebook.com</t>
+  </si>
+  <si>
+    <t>othe55555</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>100900</t>
+  </si>
+  <si>
+    <t>1-334-556-6570</t>
+  </si>
+  <si>
+    <t>1-556-778-2876</t>
+  </si>
+  <si>
+    <t>85001</t>
+  </si>
+  <si>
+    <t>1-526-272-2650</t>
+  </si>
+  <si>
+    <t>1-454-266-8970</t>
+  </si>
+  <si>
+    <t>4 Goldfield St.</t>
+  </si>
+  <si>
+    <t>70 Bowman St.</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>1-765-888-9800</t>
+  </si>
+  <si>
+    <t>1-676-999-8000</t>
+  </si>
+  <si>
+    <t>Company1</t>
+  </si>
+  <si>
+    <t>Company2</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
   </si>
 </sst>
 </file>
@@ -207,9 +258,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,51 +563,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="29" max="29" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -585,18 +638,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -608,19 +661,19 @@
         <v>500</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="L4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="M4">
         <v>2</v>
@@ -629,32 +682,32 @@
         <v>10.44444</v>
       </c>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
         <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -668,64 +721,168 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s">
+      <c r="N7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="O7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R7" t="s">
+        <v>21</v>
+      </c>
+      <c r="S7" t="s">
+        <v>61</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="J7" t="s">
+      <c r="F8" t="s">
         <v>30</v>
       </c>
-      <c r="K7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="G8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R8" t="s">
         <v>21</v>
       </c>
-      <c r="O7" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>24</v>
-      </c>
-      <c r="R7">
-        <v>411099</v>
-      </c>
-      <c r="S7" t="s">
-        <v>33</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V7">
-        <v>12345</v>
-      </c>
-      <c r="W7" t="s">
-        <v>34</v>
-      </c>
-      <c r="X7" t="s">
-        <v>35</v>
+      <c r="S8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T8" t="s">
+        <v>63</v>
+      </c>
+      <c r="U8" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added values for Vendor
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\CTPL-TestAutomation\CTPL-TestAutomation\CTPL-TestAutomation\NetConnect-NetChain2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15420" windowHeight="3945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -87,12 +92,6 @@
     <t>ltd</t>
   </si>
   <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>Maharashtra</t>
-  </si>
-  <si>
     <t>Tech Mahindra</t>
   </si>
   <si>
@@ -105,33 +104,6 @@
     <t>Ms</t>
   </si>
   <si>
-    <t>Parul</t>
-  </si>
-  <si>
-    <t>Gupta</t>
-  </si>
-  <si>
-    <t>Tata Technologies</t>
-  </si>
-  <si>
-    <t>phase3</t>
-  </si>
-  <si>
-    <t>rmhaisurkar@gmail.com</t>
-  </si>
-  <si>
-    <t>www.tata.com</t>
-  </si>
-  <si>
-    <t>notes12345</t>
-  </si>
-  <si>
-    <t>9098989912</t>
-  </si>
-  <si>
-    <t>8178789909</t>
-  </si>
-  <si>
     <t>Qwerty@123</t>
   </si>
   <si>
@@ -190,12 +162,51 @@
   </si>
   <si>
     <t>NetchainTest.CreateInvoice3</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Xyz</t>
+  </si>
+  <si>
+    <t>Company1</t>
+  </si>
+  <si>
+    <t>whc road</t>
+  </si>
+  <si>
+    <t>nagpur</t>
+  </si>
+  <si>
+    <t>mh</t>
+  </si>
+  <si>
+    <t>www.abcd.com</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>8989887677</t>
+  </si>
+  <si>
+    <t>9098987766</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>9098989988</t>
+  </si>
+  <si>
+    <t>NetchainTest.CreateVendorNeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,10 +245,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -248,6 +261,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -296,7 +312,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,9 +345,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,6 +397,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -551,40 +601,40 @@
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -614,18 +664,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -637,19 +687,19 @@
         <v>500</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M4">
         <v>33.393360000000001</v>
@@ -658,48 +708,48 @@
         <v>45.677999999999997</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="P4" t="s">
         <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="R4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="S4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -713,95 +763,193 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" t="s">
+        <v>48</v>
+      </c>
+      <c r="O9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V9">
+        <v>440015</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z9">
+        <v>12345</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" t="s">
+        <v>49</v>
+      </c>
+      <c r="P10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" t="s">
+        <v>50</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V10">
+        <v>440015</v>
+      </c>
+      <c r="W10" s="3">
+        <v>2</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z10">
+        <v>12345</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
         <v>24</v>
       </c>
-      <c r="R9">
-        <v>411099</v>
-      </c>
-      <c r="S9" t="s">
-        <v>33</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V9">
-        <v>12345</v>
-      </c>
-      <c r="W9" t="s">
-        <v>34</v>
-      </c>
-      <c r="X9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>5</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <v>200</v>
       </c>
-      <c r="J10">
+      <c r="J11">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Vendor Creation And test data
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\CTPL-TestAutomation\CTPL-TestAutomation\CTPL-TestAutomation\NetConnect-NetChain2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6285"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -204,12 +199,36 @@
   </si>
   <si>
     <t>NetChain2 – AP Vendors</t>
+  </si>
+  <si>
+    <t>NetChain2 – AP Vendor: New</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.CreateSalesOrder</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>workbooks</t>
+  </si>
+  <si>
+    <t>measure2</t>
+  </si>
+  <si>
+    <t>Bank Charges</t>
+  </si>
+  <si>
+    <t>inv desc3</t>
+  </si>
+  <si>
+    <t>measure3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +334,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,26 +367,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,23 +402,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -593,15 +578,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U4" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="29" max="29" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -730,11 +716,89 @@
       <c r="A5" t="s">
         <v>45</v>
       </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>500</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5">
+        <v>234.44444999999999</v>
+      </c>
+      <c r="N5">
+        <v>876.9757366</v>
+      </c>
     </row>
     <row r="6" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>500</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6">
+        <v>38.741129999999998</v>
+      </c>
+      <c r="N6">
+        <v>34.987736650000002</v>
+      </c>
     </row>
     <row r="7" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -838,7 +902,7 @@
         <v>54</v>
       </c>
       <c r="AC9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -960,6 +1024,17 @@
       </c>
       <c r="J11">
         <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed values in testData
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\CTPL-TestAutomation\CTPL-TestAutomation\CTPL-TestAutomation\NetConnect-NetChain2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6285"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -104,9 +99,6 @@
     <t>Ms</t>
   </si>
   <si>
-    <t>Qwerty@123</t>
-  </si>
-  <si>
     <t>Dell</t>
   </si>
   <si>
@@ -152,12 +144,6 @@
     <t>DHL</t>
   </si>
   <si>
-    <t>payable</t>
-  </si>
-  <si>
-    <t>tech m</t>
-  </si>
-  <si>
     <t>NetchainTest.CreateInvoice2</t>
   </si>
   <si>
@@ -204,12 +190,48 @@
   </si>
   <si>
     <t>NetChain2 – AP Vendors</t>
+  </si>
+  <si>
+    <t>NetChain2 – AP Vendor: New</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.CreateSalesOrder</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>measure2</t>
+  </si>
+  <si>
+    <t>Bank Charges</t>
+  </si>
+  <si>
+    <t>inv desc3</t>
+  </si>
+  <si>
+    <t>measure3</t>
+  </si>
+  <si>
+    <t>Payable</t>
+  </si>
+  <si>
+    <t>Testing1@</t>
+  </si>
+  <si>
+    <t>TechBite</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
+  </si>
+  <si>
+    <t>Account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,26 +370,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,23 +405,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -593,15 +581,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC11"/>
+  <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U4" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="29" max="29" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -609,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -620,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -631,13 +620,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -672,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -690,7 +679,7 @@
         <v>500</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -699,10 +688,10 @@
         <v>25</v>
       </c>
       <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
         <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
       </c>
       <c r="M4">
         <v>33.393360000000001</v>
@@ -711,29 +700,107 @@
         <v>45.677999999999997</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P4" t="s">
         <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="R4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>500</v>
+      </c>
+      <c r="H5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5">
+        <v>234.44444999999999</v>
+      </c>
+      <c r="N5">
+        <v>876.9757366</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>500</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6">
+        <v>38.741129999999998</v>
+      </c>
+      <c r="N6">
+        <v>34.987736650000002</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -766,16 +833,16 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
@@ -790,16 +857,16 @@
         <v>26</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q9" t="s">
         <v>22</v>
@@ -808,42 +875,42 @@
         <v>21</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V9">
         <v>440015</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Z9">
         <v>12345</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AB9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AC9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -855,16 +922,16 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
       <c r="G10" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I10" t="s">
         <v>24</v>
@@ -879,16 +946,16 @@
         <v>26</v>
       </c>
       <c r="M10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q10" t="s">
         <v>22</v>
@@ -897,13 +964,13 @@
         <v>21</v>
       </c>
       <c r="S10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="V10">
         <v>440015</v>
@@ -912,39 +979,39 @@
         <v>2</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Z10">
         <v>12345</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AB10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AC10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
@@ -960,6 +1027,17 @@
       </c>
       <c r="J11">
         <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed data in TestData for vendor
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -159,27 +159,12 @@
     <t>Company1</t>
   </si>
   <si>
-    <t>whc road</t>
-  </si>
-  <si>
-    <t>nagpur</t>
-  </si>
-  <si>
-    <t>mh</t>
-  </si>
-  <si>
     <t>www.abcd.com</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>8989887677</t>
-  </si>
-  <si>
-    <t>9098987766</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
@@ -226,6 +211,21 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>201-999-5654</t>
+  </si>
+  <si>
+    <t>210-339-0102</t>
+  </si>
+  <si>
+    <t>Street Sacramento</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Alaska</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -598,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -706,7 +706,7 @@
         <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="R4" t="s">
         <v>41</v>
@@ -720,7 +720,7 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -738,7 +738,7 @@
         <v>500</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -750,7 +750,7 @@
         <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M5">
         <v>234.44444999999999</v>
@@ -764,7 +764,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -788,13 +788,13 @@
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M6">
         <v>38.741129999999998</v>
@@ -839,10 +839,10 @@
         <v>30</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
@@ -875,42 +875,42 @@
         <v>21</v>
       </c>
       <c r="S9" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="V9">
-        <v>440015</v>
+        <v>99501</v>
       </c>
       <c r="W9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="Z9">
         <v>12345</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AB9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AC9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -928,10 +928,10 @@
         <v>30</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>24</v>
@@ -964,37 +964,37 @@
         <v>21</v>
       </c>
       <c r="S10" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="V10">
-        <v>440015</v>
+        <v>99501</v>
       </c>
       <c r="W10" s="3">
         <v>2</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="Z10">
         <v>12345</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AB10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AC10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,10 +1031,10 @@
     </row>
     <row r="13" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Changed data in testdata
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Ms</t>
   </si>
   <si>
-    <t>Qwerty@123</t>
-  </si>
-  <si>
     <t>Dell</t>
   </si>
   <si>
@@ -147,12 +144,6 @@
     <t>DHL</t>
   </si>
   <si>
-    <t>payable</t>
-  </si>
-  <si>
-    <t>tech m</t>
-  </si>
-  <si>
     <t>NetchainTest.CreateInvoice2</t>
   </si>
   <si>
@@ -168,27 +159,12 @@
     <t>Company1</t>
   </si>
   <si>
-    <t>whc road</t>
-  </si>
-  <si>
-    <t>nagpur</t>
-  </si>
-  <si>
-    <t>mh</t>
-  </si>
-  <si>
     <t>www.abcd.com</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>8989887677</t>
-  </si>
-  <si>
-    <t>9098987766</t>
-  </si>
-  <si>
     <t>Tester</t>
   </si>
   <si>
@@ -210,9 +186,6 @@
     <t>Accenture</t>
   </si>
   <si>
-    <t>workbooks</t>
-  </si>
-  <si>
     <t>measure2</t>
   </si>
   <si>
@@ -223,6 +196,36 @@
   </si>
   <si>
     <t>measure3</t>
+  </si>
+  <si>
+    <t>Payable</t>
+  </si>
+  <si>
+    <t>Testing1@</t>
+  </si>
+  <si>
+    <t>TechBite</t>
+  </si>
+  <si>
+    <t>Workbooks</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>201-999-5654</t>
+  </si>
+  <si>
+    <t>210-339-0102</t>
+  </si>
+  <si>
+    <t>Street Sacramento</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Alaska</t>
   </si>
 </sst>
 </file>
@@ -580,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -595,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -606,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -617,13 +620,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -658,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -676,7 +679,7 @@
         <v>500</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -685,10 +688,10 @@
         <v>25</v>
       </c>
       <c r="K4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
         <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
       </c>
       <c r="M4">
         <v>33.393360000000001</v>
@@ -697,27 +700,27 @@
         <v>45.677999999999997</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P4" t="s">
         <v>8</v>
       </c>
       <c r="Q4" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="R4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -735,7 +738,7 @@
         <v>500</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -744,10 +747,10 @@
         <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="M5">
         <v>234.44444999999999</v>
@@ -758,10 +761,10 @@
     </row>
     <row r="6" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -779,19 +782,19 @@
         <v>500</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="M6">
         <v>38.741129999999998</v>
@@ -830,16 +833,16 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
@@ -854,16 +857,16 @@
         <v>26</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q9" t="s">
         <v>22</v>
@@ -872,42 +875,42 @@
         <v>21</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="V9">
-        <v>440015</v>
+        <v>99501</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="Z9">
         <v>12345</v>
       </c>
       <c r="AA9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC9" t="s">
         <v>53</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -919,16 +922,16 @@
         <v>19</v>
       </c>
       <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
       <c r="G10" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I10" t="s">
         <v>24</v>
@@ -943,16 +946,16 @@
         <v>26</v>
       </c>
       <c r="M10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="O10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q10" t="s">
         <v>22</v>
@@ -961,54 +964,54 @@
         <v>21</v>
       </c>
       <c r="S10" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="V10">
-        <v>440015</v>
+        <v>99501</v>
       </c>
       <c r="W10" s="3">
         <v>2</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="Z10">
         <v>12345</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="AB10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="AC10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
@@ -1028,10 +1031,10 @@
     </row>
     <row r="13" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Runtime product addition in po & SO creation
1.Pushing the code for runtime product addition in po
2. Create SO including verification files
3.Object map file
4.Test data file
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -228,15 +228,9 @@
     <t>NetchainTest.PORuntimeProd</t>
   </si>
   <si>
-    <t>runtime prod 1</t>
-  </si>
-  <si>
     <t>new category 1</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
     <t>Installation</t>
   </si>
   <si>
@@ -274,6 +268,24 @@
   </si>
   <si>
     <t>NetchainTest.CreateSalesOrder2</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>runtime prod 17</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -631,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -709,10 +721,28 @@
         <v>69</v>
       </c>
       <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" t="s">
-        <v>71</v>
+      <c r="D4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1093,22 +1123,22 @@
         <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H14">
         <v>33.393360000000001</v>
@@ -1117,10 +1147,10 @@
         <v>45.677999999999997</v>
       </c>
       <c r="J14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L14" t="s">
         <v>63</v>
@@ -1131,25 +1161,25 @@
     </row>
     <row r="15" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H15">
         <v>25.465554999999998</v>
@@ -1160,25 +1190,25 @@
     </row>
     <row r="16" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H16">
         <v>10.44455</v>

</xml_diff>

<commit_message>
create Client and connected client testdata.
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6285"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14835" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="160">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -340,13 +341,169 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.CreateClients</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>Desire</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Shital</t>
+  </si>
+  <si>
+    <t>ruchira.mhaisurkar@connecticus.in</t>
+  </si>
+  <si>
+    <t>9876767687</t>
+  </si>
+  <si>
+    <t>desire</t>
+  </si>
+  <si>
+    <t>Fees Billed</t>
+  </si>
+  <si>
+    <t>869876986</t>
+  </si>
+  <si>
+    <t>Bank To Bank</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Patil</t>
+  </si>
+  <si>
+    <t>Nice</t>
+  </si>
+  <si>
+    <t>Company2</t>
+  </si>
+  <si>
+    <t>maharashtra</t>
+  </si>
+  <si>
+    <t>576567</t>
+  </si>
+  <si>
+    <t>ruchiramhaisurkar@connecticus.in</t>
+  </si>
+  <si>
+    <t>8768768754</t>
+  </si>
+  <si>
+    <t>4576477678</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>www.accountReceviable.com</t>
+  </si>
+  <si>
+    <t>765675753</t>
+  </si>
+  <si>
+    <t>Tier-B</t>
+  </si>
+  <si>
+    <t>NetChain2 – AR Clients</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.CreateClientsConnected</t>
+  </si>
+  <si>
+    <t>ConnectedCompany</t>
+  </si>
+  <si>
+    <t>rashmiconnecticus3@gmail.com</t>
+  </si>
+  <si>
+    <t>AP.NetchainTest.CreateVendors</t>
+  </si>
+  <si>
+    <t>Abcd</t>
+  </si>
+  <si>
+    <t>maharastra</t>
+  </si>
+  <si>
+    <t>23456</t>
+  </si>
+  <si>
+    <t>9098987766</t>
+  </si>
+  <si>
+    <t>8989887677</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>Notepads</t>
+  </si>
+  <si>
+    <t>AP.NetchainTest.CreatePO</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>Connected Ar</t>
+  </si>
+  <si>
+    <t>nice</t>
+  </si>
+  <si>
+    <t>shital</t>
+  </si>
+  <si>
+    <t>UPS Ground</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.Login</t>
+  </si>
+  <si>
+    <t>CompanyConnection</t>
+  </si>
+  <si>
+    <t>Qwerty@123</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.CreateSOConnected</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>product1</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>very nice</t>
+  </si>
+  <si>
+    <t>Rashmi</t>
+  </si>
+  <si>
+    <t>APConnected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +515,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000008"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -384,12 +548,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -695,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC18"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -729,6 +897,12 @@
       <c r="G1" t="s">
         <v>68</v>
       </c>
+      <c r="H1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="2" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1393,7 +1567,7 @@
         <v>8.3330000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1407,7 +1581,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1449,14 +1623,427 @@
       </c>
       <c r="N18" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>116</v>
+      </c>
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N19" t="s">
+        <v>118</v>
+      </c>
+      <c r="O19" t="s">
+        <v>119</v>
+      </c>
+      <c r="P19" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>120</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="T19" t="s">
+        <v>122</v>
+      </c>
+      <c r="U19" t="s">
+        <v>21</v>
+      </c>
+      <c r="V19" t="s">
+        <v>20</v>
+      </c>
+      <c r="W19" t="s">
+        <v>22</v>
+      </c>
+      <c r="X19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>116</v>
+      </c>
+      <c r="L20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N20" t="s">
+        <v>118</v>
+      </c>
+      <c r="O20" t="s">
+        <v>119</v>
+      </c>
+      <c r="P20" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>120</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S20" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="T20" t="s">
+        <v>134</v>
+      </c>
+      <c r="U20" t="s">
+        <v>21</v>
+      </c>
+      <c r="V20" t="s">
+        <v>20</v>
+      </c>
+      <c r="W20" t="s">
+        <v>22</v>
+      </c>
+      <c r="X20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC20" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" t="s">
+        <v>42</v>
+      </c>
+      <c r="N21" t="s">
+        <v>137</v>
+      </c>
+      <c r="O21" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>134</v>
+      </c>
+      <c r="R21" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T21" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="W21" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y21" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA21" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>5333.3387599999996</v>
+      </c>
+      <c r="J22">
+        <v>50.874899999999997</v>
+      </c>
+      <c r="K22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L22" t="s">
+        <v>147</v>
+      </c>
+      <c r="M22" t="s">
+        <v>148</v>
+      </c>
+      <c r="N22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:36" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" t="s">
+        <v>145</v>
+      </c>
+      <c r="H24">
+        <v>5.3453299999999997</v>
+      </c>
+      <c r="I24">
+        <v>500.34559999999999</v>
+      </c>
+      <c r="J24" t="s">
+        <v>157</v>
+      </c>
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" t="s">
+        <v>158</v>
+      </c>
+      <c r="M24" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C23" r:id="rId2"/>
+    <hyperlink ref="X21" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updating TestData.xlsx. Added data for TwoWayMatch
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="175">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -535,6 +535,12 @@
   </si>
   <si>
     <t>Send Payment</t>
+  </si>
+  <si>
+    <t>NetchainTest.TwoWayMatch1</t>
+  </si>
+  <si>
+    <t>NetchainTest.CreateInvoice4</t>
   </si>
 </sst>
 </file>
@@ -901,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ26"/>
+  <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2200,6 +2206,88 @@
       </c>
       <c r="G26" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27">
+        <v>500</v>
+      </c>
+      <c r="H27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>500</v>
+      </c>
+      <c r="H28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" t="s">
+        <v>51</v>
+      </c>
+      <c r="M28">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest test data file with CreateSO changes
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -1030,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N19" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1541,7 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
test data for setting gr custom workflow
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="191">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -586,6 +586,9 @@
   </si>
   <si>
     <t>TechBite</t>
+  </si>
+  <si>
+    <t>NetchainTest.SetGRCustomWorkflow</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL29"/>
+  <dimension ref="A1:AL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2508,6 +2511,14 @@
       <c r="AJ29" s="11"/>
       <c r="AK29" s="11"/>
       <c r="AL29" s="11"/>
+    </row>
+    <row r="30" spans="1:38" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>190</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added testdata for refund and credit memo
</commit_message>
<xml_diff>
--- a/NetConnect-NetChain2/TestData.xlsx
+++ b/NetConnect-NetChain2/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="205">
   <si>
     <t>NetchainTest.Login</t>
   </si>
@@ -579,13 +579,58 @@
     <t>NetChain2 – AP CREATE: MEMO</t>
   </si>
   <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>TechBcs</t>
   </si>
   <si>
     <t>TechBite</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.PaymentReceipt</t>
+  </si>
+  <si>
+    <t>01-30-2015</t>
+  </si>
+  <si>
+    <t>CASH</t>
+  </si>
+  <si>
+    <t>Payment desc</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
+  <si>
+    <t>AR.NetchainTest.CreateInvoice</t>
+  </si>
+  <si>
+    <t>prod_11111</t>
+  </si>
+  <si>
+    <t>Netchain.NewPurchaseOrder</t>
+  </si>
+  <si>
+    <t>description 1</t>
+  </si>
+  <si>
+    <t>Measure1</t>
+  </si>
+  <si>
+    <t>Purchase Order Approved Sucessfully</t>
+  </si>
+  <si>
+    <t>Line Saved</t>
+  </si>
+  <si>
+    <t>Vendor 3</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Processing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automationctpl8@gmail.com </t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL29"/>
+  <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.85546875" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1118,12 @@
       <c r="K1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="2"/>
+      <c r="L1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="2" spans="1:29" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2161,7 +2211,10 @@
         <v>182</v>
       </c>
       <c r="Q22" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+      <c r="R22" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:38" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2460,10 +2513,10 @@
         <v>184</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="D29" s="10">
         <v>23</v>
@@ -2509,6 +2562,159 @@
       <c r="AK29" s="11"/>
       <c r="AL29" s="11"/>
     </row>
+    <row r="30" spans="1:38" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" t="s">
+        <v>197</v>
+      </c>
+      <c r="H30" t="s">
+        <v>198</v>
+      </c>
+      <c r="I30">
+        <v>100</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+      <c r="K30" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" t="s">
+        <v>75</v>
+      </c>
+      <c r="N30" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" t="s">
+        <v>11</v>
+      </c>
+      <c r="P30" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>200</v>
+      </c>
+      <c r="R30" t="s">
+        <v>201</v>
+      </c>
+      <c r="S30">
+        <v>100</v>
+      </c>
+      <c r="T30">
+        <v>20</v>
+      </c>
+      <c r="U30">
+        <v>200</v>
+      </c>
+      <c r="V30">
+        <v>20</v>
+      </c>
+      <c r="W30">
+        <v>10</v>
+      </c>
+      <c r="X30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31">
+        <v>3454</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31">
+        <v>3243242</v>
+      </c>
+      <c r="F31" t="s">
+        <v>192</v>
+      </c>
+      <c r="G31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31">
+        <v>900</v>
+      </c>
+      <c r="I31">
+        <v>400</v>
+      </c>
+      <c r="J31" t="s">
+        <v>193</v>
+      </c>
+      <c r="K31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>194</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32">
+        <v>500.76600000000002</v>
+      </c>
+      <c r="G32" t="s">
+        <v>195</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="L32">
+        <v>500.86599999999999</v>
+      </c>
+      <c r="M32" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G29:H29"/>
@@ -2522,9 +2728,11 @@
     <hyperlink ref="K1" r:id="rId6"/>
     <hyperlink ref="E1" r:id="rId7"/>
     <hyperlink ref="E24" r:id="rId8"/>
+    <hyperlink ref="M1" r:id="rId9"/>
+    <hyperlink ref="L1" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>